<commit_message>
Update my details to the Excel file
</commit_message>
<xml_diff>
--- a/Open Source task.xlsx
+++ b/Open Source task.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\legion\Desktop\open-source\Security-Task\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\legion\Desktop\opensource\Security-Task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655120EA-671F-4435-B8F2-FC3A0DB523E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC53C2C4-32E2-4C30-8AE4-4CE7834A6F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1A782380-5C03-4ABF-949C-B3350E41F3A7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>name</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>السيد اسامه رجب السيد</t>
+  </si>
+  <si>
+    <t>Repo Link Project</t>
+  </si>
+  <si>
+    <t>https://github.com/EngNoOne/code_stego</t>
   </si>
 </sst>
 </file>
@@ -91,7 +97,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -114,15 +120,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -458,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B88C28-23A0-4FB2-A45B-5BE272931FEB}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -469,9 +487,10 @@
     <col min="1" max="1" width="46.44140625" customWidth="1"/>
     <col min="2" max="2" width="49.6640625" customWidth="1"/>
     <col min="3" max="3" width="51.6640625" customWidth="1"/>
+    <col min="4" max="4" width="38.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,8 +500,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -491,12 +513,16 @@
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{A364EA89-B4FA-4322-9DA7-87C8CDF404AF}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{65319477-3938-45F9-8CEB-9746D877D7C0}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{04D846CA-23A8-4D42-9133-D1F5365DB636}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>